<commit_message>
feat: - table order upload done
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/белье_по каждому размеру.xlsx
+++ b/app/download_dir/system_files/белье_по каждому размеру.xlsx
@@ -3159,10 +3159,10 @@
   <dimension ref="A1:AMJ1732"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G5:G1048576 G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="66.34"/>
@@ -32421,16 +32421,16 @@
       <formula1>Справочники!$I$2:$I$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G7:G1658" type="list">
-      <formula1>Справочники!$E$3:$E$112</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O7" type="list">
       <formula1>Справочники!$H$2:$H$242</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F7:F1619" type="list">
       <formula1>Справочники!$D$2:$D$33</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G5 G7:G2606" type="textLength">
+      <formula1>100</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -32452,10 +32452,10 @@
   <dimension ref="A1:I244"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="2" sqref="G5:G1048576 G6 D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -34425,10 +34425,10 @@
   <dimension ref="A1:B145"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
+      <selection pane="topLeft" activeCell="B58" activeCellId="2" sqref="G5:G1048576 G6 B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.76"/>

</xml_diff>

<commit_message>
upd:  - operator requests solved
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/белье_по каждому размеру.xlsx
+++ b/app/download_dir/system_files/белье_по каждому размеру.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2326" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2325" uniqueCount="678">
   <si>
     <t xml:space="preserve">Код ТНВЭД</t>
   </si>
@@ -579,7 +579,7 @@
     <t xml:space="preserve">МИКРОФИБРА</t>
   </si>
   <si>
-    <t xml:space="preserve">БЕЛОРУССИЯ</t>
+    <t xml:space="preserve">БЕЛАРУСЬ</t>
   </si>
   <si>
     <t xml:space="preserve">ДОРОЖКА</t>
@@ -753,7 +753,7 @@
     <t xml:space="preserve">ПОПЛИН</t>
   </si>
   <si>
-    <t xml:space="preserve">ВЕЛИКОБРИТАНИЯ</t>
+    <t xml:space="preserve">СОЕДИНЕННОЕ КОРОЛЕВСТВО</t>
   </si>
   <si>
     <t xml:space="preserve">НИКЕЛЬ</t>
@@ -1164,81 +1164,78 @@
     <t xml:space="preserve">СЕРЫЙ/ЗЕЛЕНЫЙ</t>
   </si>
   <si>
-    <t xml:space="preserve">СЕВЕРНАЯ КОРЕЯ</t>
+    <t xml:space="preserve">КОСТА-РИКА</t>
   </si>
   <si>
     <t xml:space="preserve">СИНЕ-ЗЕЛЕНЫЙ</t>
   </si>
   <si>
-    <t xml:space="preserve">КОСТА-РИКА</t>
+    <t xml:space="preserve">КОТ-Д'ИВУАР</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЛО-ГОЛУБОЙ</t>
   </si>
   <si>
-    <t xml:space="preserve">КОТ-Д'ИВУАР</t>
+    <t xml:space="preserve">КУБА</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЛО-СИНИЙ</t>
   </si>
   <si>
-    <t xml:space="preserve">КУБА</t>
+    <t xml:space="preserve">КУВЕЙТ</t>
   </si>
   <si>
     <t xml:space="preserve">СВЕТЛО-ГОЛУБОЙ</t>
   </si>
   <si>
-    <t xml:space="preserve">КУВЕЙТ</t>
+    <t xml:space="preserve">ЛАОССКАЯ НАРОДНАЯ ДЕМОКРАТИЧЕСКАЯ РЕСПУБЛИКА</t>
   </si>
   <si>
     <t xml:space="preserve">ЗЕЛЕНЫЙ МЕЛАНЖ</t>
   </si>
   <si>
-    <t xml:space="preserve">ЛАОССКАЯ НАРОДНАЯ ДЕМОКРАТИЧЕСКАЯ РЕСПУБЛИКА</t>
+    <t xml:space="preserve">ЛАТВИЯ</t>
   </si>
   <si>
     <t xml:space="preserve">ЖЕЛТЫЙ МЕЛАНЖ</t>
   </si>
   <si>
-    <t xml:space="preserve">ЛАТВИЯ</t>
+    <t xml:space="preserve">ЛЕСОТО</t>
   </si>
   <si>
     <t xml:space="preserve">СИНИЙ МЕЛАНЖ</t>
   </si>
   <si>
-    <t xml:space="preserve">ЛЕСОТО</t>
+    <t xml:space="preserve">ЛИБЕРИЯ</t>
   </si>
   <si>
     <t xml:space="preserve">КРАСНЫЙ МЕЛАНЖ</t>
   </si>
   <si>
-    <t xml:space="preserve">ЛИБЕРИЯ</t>
+    <t xml:space="preserve">ЛИВАН</t>
   </si>
   <si>
     <t xml:space="preserve">РОЗОВЫЙ МЕЛАНЖ</t>
   </si>
   <si>
-    <t xml:space="preserve">ЛИВАН</t>
+    <t xml:space="preserve">ЛИВИЯ</t>
   </si>
   <si>
     <t xml:space="preserve">ФИОЛЕТОВЫЙ МЕЛАНЖ</t>
   </si>
   <si>
-    <t xml:space="preserve">ЛИВИЯ</t>
+    <t xml:space="preserve">ЛИТВА</t>
   </si>
   <si>
     <t xml:space="preserve">ЖЕЛТО-ЗЕЛЕНЫЙ</t>
   </si>
   <si>
-    <t xml:space="preserve">ЛИТВА</t>
+    <t xml:space="preserve">ЛИХТЕНШТЕЙН</t>
   </si>
   <si>
     <t xml:space="preserve">МЕЛАНЖ</t>
   </si>
   <si>
-    <t xml:space="preserve">ЛИХТЕНШТЕЙН</t>
-  </si>
-  <si>
     <t xml:space="preserve">ЛЮКСЕМБУРГ</t>
   </si>
   <si>
@@ -1341,7 +1338,7 @@
     <t xml:space="preserve">НОРВЕГИЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">ОАЭ</t>
+    <t xml:space="preserve">ОБЪЕДИНЕННЫЕ АРАБСКИЕ ЭМИРАТЫ</t>
   </si>
   <si>
     <t xml:space="preserve">ОМАН</t>
@@ -1398,7 +1395,7 @@
     <t xml:space="preserve">РЕСПУБЛИКА КОНГО</t>
   </si>
   <si>
-    <t xml:space="preserve">ЮЖНАЯ КОРЕЯ</t>
+    <t xml:space="preserve">РЕСПУБЛИКА КОРЕЯ</t>
   </si>
   <si>
     <t xml:space="preserve">РЕСПУБЛИКА МАКЕДОНИЯ, БЫВШАЯ ЮГОСЛАВСКАЯ РЕСПУБЛИКА</t>
@@ -1470,7 +1467,7 @@
     <t xml:space="preserve">СЛОВЕНИЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">США</t>
+    <t xml:space="preserve">СОЕДИНЕННЫЕ ШТАТЫ</t>
   </si>
   <si>
     <t xml:space="preserve">СОЛОМОНОВЫ ОСТРОВА</t>
@@ -3159,10 +3156,10 @@
   <dimension ref="A1:AMJ1732"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G5:G1048576 G6"/>
+      <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="66.34"/>
@@ -32402,7 +32399,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O1199:O1606" type="list">
-      <formula1>Справочники!$H$2:$H$243</formula1>
+      <formula1>Справочники!$H$2:$H$242</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I7:I1606" type="list">
@@ -32414,7 +32411,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O8:O1198" type="list">
-      <formula1>Справочники!$H$2:$H$244</formula1>
+      <formula1>Справочники!$H$2:$H$243</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P7:P1732" type="list">
@@ -32422,7 +32419,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O7" type="list">
-      <formula1>Справочники!$H$2:$H$242</formula1>
+      <formula1>Справочники!$H$2:$H$241</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F7:F1619" type="list">
@@ -32449,13 +32446,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I244"/>
+  <dimension ref="A1:I243"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="2" sqref="G5:G1048576 G6 D15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G231" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -34393,12 +34390,7 @@
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H243" s="27" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H244" s="27"/>
+      <c r="H243" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -34425,10 +34417,10 @@
   <dimension ref="A1:B145"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B58" activeCellId="2" sqref="G5:G1048576 G6 B58"/>
+      <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.76"/>
@@ -34436,10 +34428,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
+        <v>533</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>534</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34447,7 +34439,7 @@
         <v>4203</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34455,7 +34447,7 @@
         <v>4203100001</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34463,7 +34455,7 @@
         <v>4203100009</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34471,7 +34463,7 @@
         <v>6106</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34479,7 +34471,7 @@
         <v>6106100000</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34487,7 +34479,7 @@
         <v>6106200000</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34495,7 +34487,7 @@
         <v>6106901000</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34503,7 +34495,7 @@
         <v>6106903000</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34511,7 +34503,7 @@
         <v>6106905000</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34519,7 +34511,7 @@
         <v>6106909000</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34527,7 +34519,7 @@
         <v>6201</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34535,7 +34527,7 @@
         <v>6201200000</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34543,7 +34535,7 @@
         <v>6201300000</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34551,7 +34543,7 @@
         <v>6201400000</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34559,7 +34551,7 @@
         <v>6201900000</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34567,7 +34559,7 @@
         <v>6202</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34575,7 +34567,7 @@
         <v>6202200000</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34583,7 +34575,7 @@
         <v>6202300000</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34591,7 +34583,7 @@
         <v>6202400001</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34599,7 +34591,7 @@
         <v>6202400009</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34607,7 +34599,7 @@
         <v>6202900001</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34615,7 +34607,7 @@
         <v>6202900009</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34623,7 +34615,7 @@
         <v>6302</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34631,7 +34623,7 @@
         <v>6302100001</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34639,7 +34631,7 @@
         <v>6302100009</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34647,7 +34639,7 @@
         <v>6302210000</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34655,7 +34647,7 @@
         <v>6302221000</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34663,7 +34655,7 @@
         <v>6302229000</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34671,7 +34663,7 @@
         <v>6302310001</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34679,7 +34671,7 @@
         <v>6302310009</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34687,7 +34679,7 @@
         <v>6302321000</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34695,7 +34687,7 @@
         <v>6302329000</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34703,7 +34695,7 @@
         <v>6302392001</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34711,7 +34703,7 @@
         <v>6302392009</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34719,7 +34711,7 @@
         <v>6302399000</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34727,7 +34719,7 @@
         <v>6302400000</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34735,7 +34727,7 @@
         <v>6302510001</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34743,7 +34735,7 @@
         <v>6302510009</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34751,7 +34743,7 @@
         <v>6302531000</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34759,7 +34751,7 @@
         <v>6302539000</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34767,7 +34759,7 @@
         <v>6302591000</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34775,7 +34767,7 @@
         <v>6302599000</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34783,7 +34775,7 @@
         <v>6302600000</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34791,7 +34783,7 @@
         <v>6302910000</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34799,7 +34791,7 @@
         <v>6302931000</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34807,7 +34799,7 @@
         <v>6302939000</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34815,7 +34807,7 @@
         <v>6302991000</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34823,7 +34815,7 @@
         <v>6302999000</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34831,7 +34823,7 @@
         <v>4303</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34839,7 +34831,7 @@
         <v>4303109010</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34847,7 +34839,7 @@
         <v>4303109020</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34855,7 +34847,7 @@
         <v>4303109030</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34863,7 +34855,7 @@
         <v>4303109040</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34871,7 +34863,7 @@
         <v>4303109050</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34879,7 +34871,7 @@
         <v>4303109060</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34887,7 +34879,7 @@
         <v>4303109080</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34895,7 +34887,7 @@
         <v>3303</v>
       </c>
       <c r="B58" s="36" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34903,7 +34895,7 @@
         <v>3303001000</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34911,7 +34903,7 @@
         <v>3303009000</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34919,7 +34911,7 @@
         <v>4011</v>
       </c>
       <c r="B61" s="34" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34927,7 +34919,7 @@
         <v>4011100003</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34935,7 +34927,7 @@
         <v>4011100009</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34943,7 +34935,7 @@
         <v>4011201000</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34951,7 +34943,7 @@
         <v>4011209000</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34959,7 +34951,7 @@
         <v>4011400000</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34967,7 +34959,7 @@
         <v>4011700000</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34975,7 +34967,7 @@
         <v>4011800000</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34983,7 +34975,7 @@
         <v>4011900000</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34991,7 +34983,7 @@
         <v>6401</v>
       </c>
       <c r="B70" s="34" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34999,7 +34991,7 @@
         <v>6401100000</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35007,7 +34999,7 @@
         <v>6401921000</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35015,7 +35007,7 @@
         <v>6401929000</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35023,7 +35015,7 @@
         <v>6401990000</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35031,7 +35023,7 @@
         <v>6402</v>
       </c>
       <c r="B75" s="34" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35039,7 +35031,7 @@
         <v>6402121000</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35047,7 +35039,7 @@
         <v>6402129000</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35055,7 +35047,7 @@
         <v>6402190000</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35063,7 +35055,7 @@
         <v>6402200000</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35071,7 +35063,7 @@
         <v>6402911000</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35079,7 +35071,7 @@
         <v>6402919000</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35087,7 +35079,7 @@
         <v>6402990500</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35095,7 +35087,7 @@
         <v>6402991000</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35103,7 +35095,7 @@
         <v>6402993100</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35111,7 +35103,7 @@
         <v>6402993900</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35119,7 +35111,7 @@
         <v>6402995000</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35127,7 +35119,7 @@
         <v>6402999100</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35135,7 +35127,7 @@
         <v>6402999300</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35143,7 +35135,7 @@
         <v>6402999600</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35151,7 +35143,7 @@
         <v>6402999800</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35159,7 +35151,7 @@
         <v>6403</v>
       </c>
       <c r="B91" s="34" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35167,7 +35159,7 @@
         <v>6403120000</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35175,7 +35167,7 @@
         <v>6403190000</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35183,7 +35175,7 @@
         <v>6403200000</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35191,7 +35183,7 @@
         <v>6403400000</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35199,7 +35191,7 @@
         <v>6403510500</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35207,7 +35199,7 @@
         <v>6403511100</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35215,7 +35207,7 @@
         <v>6403511500</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35223,7 +35215,7 @@
         <v>6403511900</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35231,7 +35223,7 @@
         <v>6403519100</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35239,7 +35231,7 @@
         <v>6403519500</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35247,7 +35239,7 @@
         <v>6403519900</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35255,7 +35247,7 @@
         <v>6403590500</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35263,7 +35255,7 @@
         <v>6403591100</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35271,7 +35263,7 @@
         <v>6403593100</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35279,7 +35271,7 @@
         <v>6403593500</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35287,7 +35279,7 @@
         <v>6403593900</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35295,7 +35287,7 @@
         <v>6403595000</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35303,7 +35295,7 @@
         <v>6403599100</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35311,7 +35303,7 @@
         <v>6403599500</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35319,7 +35311,7 @@
         <v>6403599900</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35327,7 +35319,7 @@
         <v>6403910500</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35335,7 +35327,7 @@
         <v>6403911100</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35343,7 +35335,7 @@
         <v>6403911300</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35351,7 +35343,7 @@
         <v>6403911600</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35359,7 +35351,7 @@
         <v>6403911800</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35367,7 +35359,7 @@
         <v>6403919100</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35375,7 +35367,7 @@
         <v>6403919300</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35383,7 +35375,7 @@
         <v>6403919600</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35391,7 +35383,7 @@
         <v>6403919800</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35399,7 +35391,7 @@
         <v>6403990500</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35407,7 +35399,7 @@
         <v>6403991100</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35415,7 +35407,7 @@
         <v>6403993100</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35423,7 +35415,7 @@
         <v>6403993300</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35431,7 +35423,7 @@
         <v>6403993600</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35439,7 +35431,7 @@
         <v>6403993800</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35447,7 +35439,7 @@
         <v>6403995000</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35455,7 +35447,7 @@
         <v>6403999100</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35463,7 +35455,7 @@
         <v>6403999300</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35471,7 +35463,7 @@
         <v>6403999600</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35479,7 +35471,7 @@
         <v>6403999800</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35487,7 +35479,7 @@
         <v>6404</v>
       </c>
       <c r="B132" s="34" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35495,7 +35487,7 @@
         <v>6404110000</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35503,7 +35495,7 @@
         <v>6404191000</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35511,7 +35503,7 @@
         <v>6404199000</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35519,7 +35511,7 @@
         <v>6404191000</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35527,7 +35519,7 @@
         <v>6404209000</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35535,7 +35527,7 @@
         <v>6405</v>
       </c>
       <c r="B138" s="34" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35543,7 +35535,7 @@
         <v>6405100001</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35551,7 +35543,7 @@
         <v>6405100009</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35559,7 +35551,7 @@
         <v>6405201000</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35567,7 +35559,7 @@
         <v>6405209100</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35575,7 +35567,7 @@
         <v>6405209900</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35583,7 +35575,7 @@
         <v>6405901000</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35591,7 +35583,7 @@
         <v>6405909000</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upd: - linen and shoes edited
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/белье_по каждому размеру.xlsx
+++ b/app/download_dir/system_files/белье_по каждому размеру.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2306" uniqueCount="662">
   <si>
     <t xml:space="preserve">Код ТНВЭД</t>
   </si>
@@ -282,7 +282,7 @@
     <t xml:space="preserve">Значение атрибута</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОДОДЕЯЛЬНИК С ВЫРЕЗОМ</t>
+    <t xml:space="preserve">ПРОСТЫНЯ</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЖЕВЫЙ МЕЛАНЖ</t>
@@ -297,9 +297,6 @@
     <t xml:space="preserve">АВСТРАЛИЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОДОДЕЯЛЬНИК С КЛАПАНОМ</t>
-  </si>
-  <si>
     <t xml:space="preserve">БЕЖЕВЫЙ/ЗЕЛЕНЫЙ</t>
   </si>
   <si>
@@ -312,7 +309,7 @@
     <t xml:space="preserve">АВСТРИЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОДЗОР</t>
+    <t xml:space="preserve">НАМАТРАСНИК</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЖЕВЫЙ/СИНИЙ</t>
@@ -330,7 +327,7 @@
     <t xml:space="preserve">Модель</t>
   </si>
   <si>
-    <t xml:space="preserve">ПРОСТЫНЯ</t>
+    <t xml:space="preserve">КОМПЛЕКТ ПОСТЕЛЬНОГО БЕЛЬЯ</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЛО-ЗЕЛЕНЫЙ</t>
@@ -342,6 +339,9 @@
     <t xml:space="preserve">АЛАНДСКИЕ ОСТРОВА</t>
   </si>
   <si>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ ГОСТЕВОЕ</t>
+  </si>
+  <si>
     <t xml:space="preserve">БЕЛО-КОРИЧНЕВЫЙ</t>
   </si>
   <si>
@@ -354,7 +354,7 @@
     <t xml:space="preserve">Модель / Артикул</t>
   </si>
   <si>
-    <t xml:space="preserve">НАМАТРАСНИК</t>
+    <t xml:space="preserve">КОМПЛЕКТ ПОЛОТЕНЕЦ</t>
   </si>
   <si>
     <t xml:space="preserve">БИОМАТИН</t>
@@ -363,7 +363,7 @@
     <t xml:space="preserve">АЛЖИР</t>
   </si>
   <si>
-    <t xml:space="preserve">НАВОЛОЧКА КВАДРАТНАЯ</t>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ БАННОЕ/КУПАЛЬНОЕ ПОЛОТЕНЦЕ</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЛЫЙ</t>
@@ -375,7 +375,7 @@
     <t xml:space="preserve">АМЕРИКАНСКИЕ ВИРГИНСКИЕ ОСТРОВА</t>
   </si>
   <si>
-    <t xml:space="preserve">НАВОЛОЧКА ПРЯМОУГОЛЬНАЯ</t>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ ДЛЯ РУК</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЛЫЙ/БЕЖЕВЫЙ</t>
@@ -387,7 +387,7 @@
     <t xml:space="preserve">АМЕРИКАНСКОЕ САМОА</t>
   </si>
   <si>
-    <t xml:space="preserve">НАВОЛОЧКА ЦИЛИНДРИЧЕСКАЯ</t>
+    <t xml:space="preserve">ПОЛОТЕНЦЕ ПЛЯЖНОЕ</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЛЫЙ/СЕРЫЙ</t>
@@ -399,7 +399,7 @@
     <t xml:space="preserve">АНГИЛЬЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">КОМПЛЕКТ ПОСТЕЛЬНОГО БЕЛЬЯ</t>
+    <t xml:space="preserve">КОВРИК</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЛЫЙ/СИНИЙ</t>
@@ -411,7 +411,7 @@
     <t xml:space="preserve">АНГОЛА</t>
   </si>
   <si>
-    <t xml:space="preserve">КОМПЛЕКТ ПОЛОТЕНЕЦ</t>
+    <t xml:space="preserve">ИЗДЕЛИЕ ДЛЯ БАНИ И САУНЫ</t>
   </si>
   <si>
     <t xml:space="preserve">БИРЮЗОВЫЙ</t>
@@ -423,7 +423,7 @@
     <t xml:space="preserve">АНДОРРА</t>
   </si>
   <si>
-    <t xml:space="preserve">ГОСТЕВОЕ ПОЛОТЕНЦЕ ДЛЯ РУК</t>
+    <t xml:space="preserve">ДОРОЖКА</t>
   </si>
   <si>
     <t xml:space="preserve">БОРДОВО-РЫЖИЙ</t>
@@ -435,7 +435,7 @@
     <t xml:space="preserve">АНТАРКТИДА</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОЛОТЕНЦЕ БАННОЕ/КУПАЛЬНОЕ ПОЛОТЕНЦЕ</t>
+    <t xml:space="preserve">САЛФЕТКА ПОД ПРИБОРЫ</t>
   </si>
   <si>
     <t xml:space="preserve">БОРДОВЫЙ</t>
@@ -453,7 +453,7 @@
     <t xml:space="preserve">ТР ТС 007/2011 "О безопасности продукции, предназначенной для детей и подростков"</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОЛОТЕНЦЕ ДЛЯ ПУТЕШЕСТВИЙ</t>
+    <t xml:space="preserve">САЛФЕТКА</t>
   </si>
   <si>
     <t xml:space="preserve">БРОНЗОВЫЙ</t>
@@ -468,7 +468,7 @@
     <t xml:space="preserve">ТР ТС 017/2011 "О безопасности продукции легкой промышленности"</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОЛОТЕНЦЕ ДЛЯ РУК</t>
+    <t xml:space="preserve">СКАТЕРТЬ</t>
   </si>
   <si>
     <t xml:space="preserve">ВАНИЛЬ</t>
@@ -483,9 +483,6 @@
     <t xml:space="preserve">ТР ТС 005/2011 "О безопасности упаковки"</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОЛОТЕНЦЕ КУХОННОЕ ДЛЯ СУШКИ</t>
-  </si>
-  <si>
     <t xml:space="preserve">ВИШНЯ</t>
   </si>
   <si>
@@ -498,9 +495,6 @@
     <t xml:space="preserve">Действие технических регламентов не распространяется</t>
   </si>
   <si>
-    <t xml:space="preserve">ТРЯПКА ДЛЯ МЫТЬЯ ПОСУДЫ</t>
-  </si>
-  <si>
     <t xml:space="preserve">ГОЛУБОЙ</t>
   </si>
   <si>
@@ -510,9 +504,6 @@
     <t xml:space="preserve">АФГАНИСТАН</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОЛОТЕНЦА ПЛЯЖНЫЕ</t>
-  </si>
-  <si>
     <t xml:space="preserve">ГОРЧИЧНЫЙ</t>
   </si>
   <si>
@@ -522,9 +513,6 @@
     <t xml:space="preserve">БАГАМЫ</t>
   </si>
   <si>
-    <t xml:space="preserve">КОВРИК</t>
-  </si>
-  <si>
     <t xml:space="preserve">ГРАФИТОВЫЙ</t>
   </si>
   <si>
@@ -534,9 +522,6 @@
     <t xml:space="preserve">БАНГЛАДЕШ</t>
   </si>
   <si>
-    <t xml:space="preserve">ИЗДЕЛИЯ ДЛЯ САУНЫ</t>
-  </si>
-  <si>
     <t xml:space="preserve">ЖЁЛТЫЙ</t>
   </si>
   <si>
@@ -546,9 +531,6 @@
     <t xml:space="preserve">БАРБАДОС</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОЛОТЕНЦЕ ДЛЯ ЧАЙНОЙ ПОСУДЫ</t>
-  </si>
-  <si>
     <t xml:space="preserve">ЗЕЛЁНЫЙ</t>
   </si>
   <si>
@@ -558,9 +540,6 @@
     <t xml:space="preserve">БАХРЕЙН</t>
   </si>
   <si>
-    <t xml:space="preserve">АЖУРНАЯ САЛФЕТКА/САЛФЕТКА ПОД ПРИБОРЫ</t>
-  </si>
-  <si>
     <t xml:space="preserve">ЗОЛОТИСТЫЙ</t>
   </si>
   <si>
@@ -570,9 +549,6 @@
     <t xml:space="preserve">БЕЛИЗ</t>
   </si>
   <si>
-    <t xml:space="preserve">ДОРОЖКА</t>
-  </si>
-  <si>
     <t xml:space="preserve">ЗОЛОТОЙ</t>
   </si>
   <si>
@@ -582,9 +558,6 @@
     <t xml:space="preserve">БЕЛАРУСЬ</t>
   </si>
   <si>
-    <t xml:space="preserve">КОМПЛЕКТ СТОЛОВОГО БЕЛЬЯ</t>
-  </si>
-  <si>
     <t xml:space="preserve">ИЗУМРУДНЫЙ</t>
   </si>
   <si>
@@ -594,9 +567,6 @@
     <t xml:space="preserve">БЕЛЬГИЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОКРЫТИЕ ДЛЯ ПОДУШЕК</t>
-  </si>
-  <si>
     <t xml:space="preserve">КАПУЧИНО</t>
   </si>
   <si>
@@ -606,9 +576,6 @@
     <t xml:space="preserve">БЕНИН</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОКРЫТИЕ ДЛЯ СТУЛА</t>
-  </si>
-  <si>
     <t xml:space="preserve">КИРПИЧНЫЙ</t>
   </si>
   <si>
@@ -618,9 +585,6 @@
     <t xml:space="preserve">БЕРМУДЫ</t>
   </si>
   <si>
-    <t xml:space="preserve">ПОКРЫТИЯ ДЛЯ ДИВАНОВ</t>
-  </si>
-  <si>
     <t xml:space="preserve">КОРАЛЛОВЫЙ</t>
   </si>
   <si>
@@ -630,9 +594,6 @@
     <t xml:space="preserve">БОЛГАРИЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">САЛФЕТКА ПОД ПРИБОРЫ (МНОГОРАЗОВАЯ)</t>
-  </si>
-  <si>
     <t xml:space="preserve">КОРИЧНЕВЫЙ</t>
   </si>
   <si>
@@ -642,16 +603,10 @@
     <t xml:space="preserve">БОЛИВИЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">САЛФЕТКИ (МНОГОРАЗОВЫЕ)</t>
-  </si>
-  <si>
     <t xml:space="preserve">ПЕРИОТЕК</t>
   </si>
   <si>
     <t xml:space="preserve">БОСНИЯ И ГЕРЦЕГОВИНА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СКАТЕРТЬ (МНОГОРАЗОВАЯ)</t>
   </si>
   <si>
     <t xml:space="preserve">КРАСНО-КОРИЧНЕВЫЙ</t>
@@ -3147,10 +3102,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="65.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="65.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="47.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="27.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="34.53"/>
@@ -32434,11 +32389,11 @@
   </sheetPr>
   <dimension ref="A1:I243"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="24.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="49.34"/>
@@ -32522,19 +32477,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="26" t="s">
         <v>92</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>93</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>73</v>
@@ -32542,50 +32497,50 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>56</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="26" t="s">
         <v>102</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>104</v>
@@ -32599,7 +32554,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>107</v>
@@ -32762,17 +32717,14 @@
       <c r="B18" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="H18" s="26" t="s">
         <v>153</v>
-      </c>
-      <c r="H18" s="26" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32780,712 +32732,670 @@
         <v>139</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="H19" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="G19" s="7" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="H19" s="26" t="s">
+      <c r="G20" s="7" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="7" t="s">
+      <c r="H20" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="E20" s="7" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="H20" s="26" t="s">
+      <c r="H21" s="26" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="7" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="H22" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="H21" s="26" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="7" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="H23" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="G22" s="7" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="H22" s="26" t="s">
+      <c r="G24" s="7" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="7" t="s">
+      <c r="H24" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="E23" s="7" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="H25" s="26" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="7" t="s">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="G26" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="H26" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="H24" s="26" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="7" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="H27" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="G25" s="7" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="H25" s="26" t="s">
+      <c r="G28" s="7" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="7" t="s">
+      <c r="H28" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="E26" s="7" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="H26" s="26" t="s">
+      <c r="H29" s="26" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="7" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="G30" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="H30" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="H27" s="26" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="H28" s="26" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="H29" s="26" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="H30" s="26" t="s">
-        <v>203</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="7" t="s">
-        <v>204</v>
-      </c>
       <c r="E31" s="7" t="s">
         <v>54</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="H31" s="26" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="7" t="s">
-        <v>207</v>
-      </c>
       <c r="E32" s="7" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="H32" s="26" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="0"/>
       <c r="E33" s="7" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="H33" s="26" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="7" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="H34" s="26" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="7" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="H35" s="26" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="7" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="H36" s="26" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="7" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="H37" s="26" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="7" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="H38" s="26" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="7" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="H39" s="26" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E40" s="7" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="H40" s="26" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E41" s="7" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="H41" s="26" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="7" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="H42" s="26" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="7" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="H43" s="26" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="7" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="H44" s="26" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="7" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="H45" s="26" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="7" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H46" s="26" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E47" s="7" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="H47" s="26" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="7" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="H48" s="26" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E49" s="7" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="H49" s="26" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="7" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="H50" s="26" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="7" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="H51" s="26" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="7" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="H52" s="26" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="7" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="7" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="7" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E56" s="7" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="7" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="7" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="7" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="7" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="7" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="H61" s="26" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="7" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="H62" s="26" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="7" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="H63" s="26" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="7" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="H64" s="26" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="7" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="H65" s="26" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E66" s="7" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="H66" s="26" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="7" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="H67" s="26" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="7" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="H68" s="26" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E69" s="7" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="H69" s="26" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="7" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="H70" s="26" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E71" s="7" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="H71" s="26" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="7" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="H72" s="26" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="7" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="H73" s="26" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="7" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="H74" s="26" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E75" s="7" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="H75" s="26" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="7" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="H76" s="26" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E77" s="7" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="H77" s="26" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E78" s="7" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="H78" s="26" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E79" s="7" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="H79" s="26" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="7" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="H80" s="26" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E81" s="7" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="H81" s="26" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E82" s="7" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="H82" s="26" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="7" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="H83" s="26" t="s">
         <v>72</v>
@@ -33493,103 +33403,103 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E84" s="7" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="H84" s="26" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E85" s="7" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="H85" s="26" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E86" s="7" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="H86" s="26" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="7" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="H87" s="26" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E88" s="7" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="H88" s="26" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E89" s="7" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="H89" s="26" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E90" s="7" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="H90" s="26" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E91" s="7" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="H91" s="26" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E92" s="7" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="H92" s="26" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E93" s="7" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="H93" s="26" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="7" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="H94" s="26" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E95" s="7" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="H95" s="26" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E96" s="7" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="H96" s="26" t="s">
         <v>61</v>
@@ -33597,774 +33507,774 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E97" s="7" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="H97" s="26" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E98" s="7" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="H98" s="26" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E99" s="7" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="H99" s="26" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="7" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="H100" s="26" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E101" s="7" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="H101" s="26" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E102" s="7" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="H102" s="26" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E103" s="7" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="H103" s="26" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E104" s="7" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="H104" s="26" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E105" s="7" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="H105" s="26" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E106" s="7" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="H106" s="26" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E107" s="7" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="H107" s="26" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E108" s="7" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="H108" s="26" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="7" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="H109" s="26" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E110" s="7" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="H110" s="26" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H111" s="26" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H112" s="26" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H113" s="26" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H114" s="26" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H115" s="26" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H116" s="26" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H117" s="26" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H118" s="26" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H119" s="26" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H120" s="26" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H121" s="26" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H122" s="26" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H123" s="26" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H124" s="26" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H125" s="26" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H126" s="26" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H127" s="26" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H128" s="26" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H129" s="26" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H130" s="26" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H131" s="26" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H132" s="26" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H133" s="26" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H134" s="26" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H135" s="26" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H136" s="26" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H137" s="26" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H138" s="26" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H139" s="26" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H140" s="26" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H141" s="26" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H142" s="26" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H143" s="26" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H144" s="26" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H145" s="26" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H146" s="26" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H147" s="26" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H148" s="26" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H149" s="26" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H150" s="26" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H151" s="26" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H152" s="26" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H153" s="26" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H154" s="26" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H155" s="26" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H156" s="26" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H157" s="26" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H158" s="26" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H159" s="26" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H160" s="26" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H161" s="26" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H162" s="26" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H163" s="26" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H164" s="26" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H165" s="26" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H166" s="26" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H167" s="26" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H168" s="26" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H169" s="26" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H170" s="26" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H171" s="26" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H172" s="26" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H173" s="26" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H174" s="26" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H175" s="26" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H176" s="26" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H177" s="26" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H178" s="26" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H179" s="26" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H180" s="26" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H181" s="26" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H182" s="26" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H183" s="26" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H184" s="26" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H185" s="26" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H186" s="26" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H187" s="26" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H188" s="26" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H189" s="26" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H190" s="26" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H191" s="26" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H192" s="26" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H193" s="26" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H194" s="26" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H195" s="26" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H196" s="26" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H197" s="26" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H198" s="26" t="s">
-        <v>487</v>
+        <v>472</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H199" s="26" t="s">
-        <v>488</v>
+        <v>473</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H200" s="26" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H201" s="26" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H202" s="26" t="s">
-        <v>491</v>
+        <v>476</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H203" s="26" t="s">
-        <v>492</v>
+        <v>477</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H204" s="26" t="s">
-        <v>493</v>
+        <v>478</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H205" s="26" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H206" s="26" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H207" s="26" t="s">
-        <v>496</v>
+        <v>481</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H208" s="26" t="s">
-        <v>497</v>
+        <v>482</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H209" s="26" t="s">
-        <v>498</v>
+        <v>483</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H210" s="26" t="s">
-        <v>499</v>
+        <v>484</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H211" s="26" t="s">
-        <v>500</v>
+        <v>485</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H212" s="26" t="s">
-        <v>501</v>
+        <v>486</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H213" s="26" t="s">
-        <v>502</v>
+        <v>487</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H214" s="26" t="s">
-        <v>503</v>
+        <v>488</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H215" s="26" t="s">
-        <v>504</v>
+        <v>489</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H216" s="26" t="s">
-        <v>505</v>
+        <v>490</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H217" s="26" t="s">
-        <v>506</v>
+        <v>491</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H218" s="26" t="s">
-        <v>507</v>
+        <v>492</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H219" s="26" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H220" s="26" t="s">
-        <v>509</v>
+        <v>494</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H221" s="26" t="s">
-        <v>510</v>
+        <v>495</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H222" s="26" t="s">
-        <v>511</v>
+        <v>496</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H223" s="26" t="s">
-        <v>512</v>
+        <v>497</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H224" s="26" t="s">
-        <v>513</v>
+        <v>498</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H225" s="26" t="s">
-        <v>514</v>
+        <v>499</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H226" s="26" t="s">
-        <v>515</v>
+        <v>500</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H227" s="26" t="s">
-        <v>516</v>
+        <v>501</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H228" s="26" t="s">
-        <v>517</v>
+        <v>502</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H229" s="26" t="s">
-        <v>518</v>
+        <v>503</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H230" s="26" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H231" s="26" t="s">
-        <v>520</v>
+        <v>505</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H232" s="26" t="s">
-        <v>521</v>
+        <v>506</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H233" s="26" t="s">
-        <v>522</v>
+        <v>507</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H234" s="26" t="s">
-        <v>523</v>
+        <v>508</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H235" s="26" t="s">
-        <v>524</v>
+        <v>509</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H236" s="26" t="s">
-        <v>525</v>
+        <v>510</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H237" s="26" t="s">
-        <v>526</v>
+        <v>511</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H238" s="26" t="s">
-        <v>527</v>
+        <v>512</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H239" s="26" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H240" s="26" t="s">
-        <v>529</v>
+        <v>514</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H241" s="26" t="s">
-        <v>530</v>
+        <v>515</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H242" s="26" t="s">
-        <v>531</v>
+        <v>516</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34398,7 +34308,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.06640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="53.04"/>
@@ -34406,10 +34316,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>532</v>
+        <v>517</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>533</v>
+        <v>518</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34417,7 +34327,7 @@
         <v>4203</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34425,7 +34335,7 @@
         <v>4203100001</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34433,7 +34343,7 @@
         <v>4203100009</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34441,7 +34351,7 @@
         <v>6106</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>537</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34449,7 +34359,7 @@
         <v>6106100000</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>538</v>
+        <v>523</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34457,7 +34367,7 @@
         <v>6106200000</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>539</v>
+        <v>524</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34465,7 +34375,7 @@
         <v>6106901000</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>540</v>
+        <v>525</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34473,7 +34383,7 @@
         <v>6106903000</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>541</v>
+        <v>526</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34481,7 +34391,7 @@
         <v>6106905000</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>542</v>
+        <v>527</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34489,7 +34399,7 @@
         <v>6106909000</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>543</v>
+        <v>528</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34497,7 +34407,7 @@
         <v>6201</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>544</v>
+        <v>529</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34505,7 +34415,7 @@
         <v>6201200000</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>545</v>
+        <v>530</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34513,7 +34423,7 @@
         <v>6201300000</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>546</v>
+        <v>531</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34521,7 +34431,7 @@
         <v>6201400000</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>547</v>
+        <v>532</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34529,7 +34439,7 @@
         <v>6201900000</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>548</v>
+        <v>533</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34537,7 +34447,7 @@
         <v>6202</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>549</v>
+        <v>534</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34545,7 +34455,7 @@
         <v>6202200000</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34553,7 +34463,7 @@
         <v>6202300000</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34561,7 +34471,7 @@
         <v>6202400001</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>552</v>
+        <v>537</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34569,7 +34479,7 @@
         <v>6202400009</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>553</v>
+        <v>538</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34577,7 +34487,7 @@
         <v>6202900001</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>554</v>
+        <v>539</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34585,7 +34495,7 @@
         <v>6202900009</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>555</v>
+        <v>540</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34593,7 +34503,7 @@
         <v>6302</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>556</v>
+        <v>541</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34601,7 +34511,7 @@
         <v>6302100001</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>557</v>
+        <v>542</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34609,7 +34519,7 @@
         <v>6302100009</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>558</v>
+        <v>543</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34617,7 +34527,7 @@
         <v>6302210000</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>559</v>
+        <v>544</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34625,7 +34535,7 @@
         <v>6302221000</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>560</v>
+        <v>545</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34633,7 +34543,7 @@
         <v>6302229000</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>561</v>
+        <v>546</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34641,7 +34551,7 @@
         <v>6302310001</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>562</v>
+        <v>547</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34649,7 +34559,7 @@
         <v>6302310009</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>563</v>
+        <v>548</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34657,7 +34567,7 @@
         <v>6302321000</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>564</v>
+        <v>549</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34665,7 +34575,7 @@
         <v>6302329000</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>565</v>
+        <v>550</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34673,7 +34583,7 @@
         <v>6302392001</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>566</v>
+        <v>551</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34681,7 +34591,7 @@
         <v>6302392009</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>567</v>
+        <v>552</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34689,7 +34599,7 @@
         <v>6302399000</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34697,7 +34607,7 @@
         <v>6302400000</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34705,7 +34615,7 @@
         <v>6302510001</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>570</v>
+        <v>555</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34713,7 +34623,7 @@
         <v>6302510009</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>571</v>
+        <v>556</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34721,7 +34631,7 @@
         <v>6302531000</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>572</v>
+        <v>557</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34729,7 +34639,7 @@
         <v>6302539000</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>573</v>
+        <v>558</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34737,7 +34647,7 @@
         <v>6302591000</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>574</v>
+        <v>559</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34745,7 +34655,7 @@
         <v>6302599000</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>575</v>
+        <v>560</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34753,7 +34663,7 @@
         <v>6302600000</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>576</v>
+        <v>561</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34761,7 +34671,7 @@
         <v>6302910000</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>577</v>
+        <v>562</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34769,7 +34679,7 @@
         <v>6302931000</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>578</v>
+        <v>563</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34777,7 +34687,7 @@
         <v>6302939000</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>579</v>
+        <v>564</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34785,7 +34695,7 @@
         <v>6302991000</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>580</v>
+        <v>565</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34793,7 +34703,7 @@
         <v>6302999000</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>581</v>
+        <v>566</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34801,7 +34711,7 @@
         <v>4303</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34809,7 +34719,7 @@
         <v>4303109010</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>583</v>
+        <v>568</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34817,7 +34727,7 @@
         <v>4303109020</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>584</v>
+        <v>569</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34825,7 +34735,7 @@
         <v>4303109030</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>585</v>
+        <v>570</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34833,7 +34743,7 @@
         <v>4303109040</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>586</v>
+        <v>571</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34841,7 +34751,7 @@
         <v>4303109050</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>587</v>
+        <v>572</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34849,7 +34759,7 @@
         <v>4303109060</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>588</v>
+        <v>573</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34857,7 +34767,7 @@
         <v>4303109080</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>589</v>
+        <v>574</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34865,7 +34775,7 @@
         <v>3303</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>590</v>
+        <v>575</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34873,7 +34783,7 @@
         <v>3303001000</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>591</v>
+        <v>576</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34881,7 +34791,7 @@
         <v>3303009000</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>592</v>
+        <v>577</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34889,7 +34799,7 @@
         <v>4011</v>
       </c>
       <c r="B61" s="33" t="s">
-        <v>593</v>
+        <v>578</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34897,7 +34807,7 @@
         <v>4011100003</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>594</v>
+        <v>579</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34905,7 +34815,7 @@
         <v>4011100009</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>595</v>
+        <v>580</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34913,7 +34823,7 @@
         <v>4011201000</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>596</v>
+        <v>581</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34921,7 +34831,7 @@
         <v>4011209000</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>597</v>
+        <v>582</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34929,7 +34839,7 @@
         <v>4011400000</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>598</v>
+        <v>583</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34937,7 +34847,7 @@
         <v>4011700000</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>599</v>
+        <v>584</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34945,7 +34855,7 @@
         <v>4011800000</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>600</v>
+        <v>585</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34953,7 +34863,7 @@
         <v>4011900000</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>601</v>
+        <v>586</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34961,7 +34871,7 @@
         <v>6401</v>
       </c>
       <c r="B70" s="33" t="s">
-        <v>602</v>
+        <v>587</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34969,7 +34879,7 @@
         <v>6401100000</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>603</v>
+        <v>588</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34977,7 +34887,7 @@
         <v>6401921000</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>604</v>
+        <v>589</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34985,7 +34895,7 @@
         <v>6401929000</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>605</v>
+        <v>590</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34993,7 +34903,7 @@
         <v>6401990000</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>606</v>
+        <v>591</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35001,7 +34911,7 @@
         <v>6402</v>
       </c>
       <c r="B75" s="33" t="s">
-        <v>607</v>
+        <v>592</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35009,7 +34919,7 @@
         <v>6402121000</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>608</v>
+        <v>593</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35017,7 +34927,7 @@
         <v>6402129000</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>609</v>
+        <v>594</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35025,7 +34935,7 @@
         <v>6402190000</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>610</v>
+        <v>595</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35033,7 +34943,7 @@
         <v>6402200000</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>611</v>
+        <v>596</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35041,7 +34951,7 @@
         <v>6402911000</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>612</v>
+        <v>597</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35049,7 +34959,7 @@
         <v>6402919000</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>613</v>
+        <v>598</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35057,7 +34967,7 @@
         <v>6402990500</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>614</v>
+        <v>599</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35065,7 +34975,7 @@
         <v>6402991000</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>615</v>
+        <v>600</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35073,7 +34983,7 @@
         <v>6402993100</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>616</v>
+        <v>601</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35081,7 +34991,7 @@
         <v>6402993900</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>617</v>
+        <v>602</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35089,7 +34999,7 @@
         <v>6402995000</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>618</v>
+        <v>603</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35097,7 +35007,7 @@
         <v>6402999100</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>619</v>
+        <v>604</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35105,7 +35015,7 @@
         <v>6402999300</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>620</v>
+        <v>605</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35113,7 +35023,7 @@
         <v>6402999600</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>621</v>
+        <v>606</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35121,7 +35031,7 @@
         <v>6402999800</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>621</v>
+        <v>606</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35129,7 +35039,7 @@
         <v>6403</v>
       </c>
       <c r="B91" s="33" t="s">
-        <v>622</v>
+        <v>607</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35137,7 +35047,7 @@
         <v>6403120000</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>623</v>
+        <v>608</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35145,7 +35055,7 @@
         <v>6403190000</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>624</v>
+        <v>609</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35153,7 +35063,7 @@
         <v>6403200000</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>625</v>
+        <v>610</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35161,7 +35071,7 @@
         <v>6403400000</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>626</v>
+        <v>611</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35169,7 +35079,7 @@
         <v>6403510500</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>627</v>
+        <v>612</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35177,7 +35087,7 @@
         <v>6403511100</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>628</v>
+        <v>613</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35185,7 +35095,7 @@
         <v>6403511500</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>629</v>
+        <v>614</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35193,7 +35103,7 @@
         <v>6403511900</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>630</v>
+        <v>615</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35201,7 +35111,7 @@
         <v>6403519100</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>631</v>
+        <v>616</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35209,7 +35119,7 @@
         <v>6403519500</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35217,7 +35127,7 @@
         <v>6403519900</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>633</v>
+        <v>618</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35225,7 +35135,7 @@
         <v>6403590500</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>634</v>
+        <v>619</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35233,7 +35143,7 @@
         <v>6403591100</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>635</v>
+        <v>620</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35241,7 +35151,7 @@
         <v>6403593100</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35249,7 +35159,7 @@
         <v>6403593500</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>637</v>
+        <v>622</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35257,7 +35167,7 @@
         <v>6403593900</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>638</v>
+        <v>623</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35265,7 +35175,7 @@
         <v>6403595000</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>639</v>
+        <v>624</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35273,7 +35183,7 @@
         <v>6403599100</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>640</v>
+        <v>625</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35281,7 +35191,7 @@
         <v>6403599500</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>641</v>
+        <v>626</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35289,7 +35199,7 @@
         <v>6403599900</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>642</v>
+        <v>627</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35297,7 +35207,7 @@
         <v>6403910500</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>643</v>
+        <v>628</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35305,7 +35215,7 @@
         <v>6403911100</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>644</v>
+        <v>629</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35313,7 +35223,7 @@
         <v>6403911300</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>645</v>
+        <v>630</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35321,7 +35231,7 @@
         <v>6403911600</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>646</v>
+        <v>631</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35329,7 +35239,7 @@
         <v>6403911800</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>647</v>
+        <v>632</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35337,7 +35247,7 @@
         <v>6403919100</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>648</v>
+        <v>633</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35345,7 +35255,7 @@
         <v>6403919300</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>649</v>
+        <v>634</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35353,7 +35263,7 @@
         <v>6403919600</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>650</v>
+        <v>635</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35361,7 +35271,7 @@
         <v>6403919800</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>651</v>
+        <v>636</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35369,7 +35279,7 @@
         <v>6403990500</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>652</v>
+        <v>637</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35377,7 +35287,7 @@
         <v>6403991100</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>653</v>
+        <v>638</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35385,7 +35295,7 @@
         <v>6403993100</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>654</v>
+        <v>639</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35393,7 +35303,7 @@
         <v>6403993300</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>655</v>
+        <v>640</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35401,7 +35311,7 @@
         <v>6403993600</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>656</v>
+        <v>641</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35409,7 +35319,7 @@
         <v>6403993800</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>657</v>
+        <v>642</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35417,7 +35327,7 @@
         <v>6403995000</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>658</v>
+        <v>643</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35425,7 +35335,7 @@
         <v>6403999100</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>659</v>
+        <v>644</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35433,7 +35343,7 @@
         <v>6403999300</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>660</v>
+        <v>645</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35441,7 +35351,7 @@
         <v>6403999600</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>661</v>
+        <v>646</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35449,7 +35359,7 @@
         <v>6403999800</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>662</v>
+        <v>647</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35457,7 +35367,7 @@
         <v>6404</v>
       </c>
       <c r="B132" s="33" t="s">
-        <v>663</v>
+        <v>648</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35465,7 +35375,7 @@
         <v>6404110000</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>664</v>
+        <v>649</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35473,7 +35383,7 @@
         <v>6404191000</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>665</v>
+        <v>650</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35481,7 +35391,7 @@
         <v>6404199000</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>666</v>
+        <v>651</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35489,7 +35399,7 @@
         <v>6404191000</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>667</v>
+        <v>652</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35497,7 +35407,7 @@
         <v>6404209000</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>668</v>
+        <v>653</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35505,7 +35415,7 @@
         <v>6405</v>
       </c>
       <c r="B138" s="33" t="s">
-        <v>669</v>
+        <v>654</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35513,7 +35423,7 @@
         <v>6405100001</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>670</v>
+        <v>655</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35521,7 +35431,7 @@
         <v>6405100009</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>671</v>
+        <v>656</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35529,7 +35439,7 @@
         <v>6405201000</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>672</v>
+        <v>657</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35537,7 +35447,7 @@
         <v>6405209100</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>673</v>
+        <v>658</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35545,7 +35455,7 @@
         <v>6405209900</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>674</v>
+        <v>659</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35553,7 +35463,7 @@
         <v>6405901000</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35561,7 +35471,7 @@
         <v>6405909000</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>676</v>
+        <v>661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upd: - colors edit - tnved clothes common МАЙКА edit
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/белье_по каждому размеру.xlsx
+++ b/app/download_dir/system_files/белье_по каждому размеру.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="689">
   <si>
     <t xml:space="preserve">Код ТНВЭД</t>
   </si>
@@ -1260,7 +1260,13 @@
     <t xml:space="preserve">ЛИТВА</t>
   </si>
   <si>
+    <t xml:space="preserve">СЕРО-ЗЕЛЕНЫЙ</t>
+  </si>
+  <si>
     <t xml:space="preserve">ЛИХТЕНШТЕЙН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СЕРО-ЗЕЛЁНЫЙ</t>
   </si>
   <si>
     <t xml:space="preserve">ЛЮКСЕМБУРГ</t>
@@ -3167,10 +3173,10 @@
   <dimension ref="A1:AMJ1780"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="65.42"/>
@@ -32714,11 +32720,11 @@
   </sheetPr>
   <dimension ref="A1:I243"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E111" activeCellId="0" sqref="E111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="24.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="49.34"/>
@@ -34014,663 +34020,669 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E111" s="7" t="s">
+        <v>410</v>
+      </c>
       <c r="H111" s="26" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E112" s="7" t="s">
+        <v>412</v>
+      </c>
       <c r="H112" s="26" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H113" s="26" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H114" s="26" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H115" s="26" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H116" s="26" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H117" s="26" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H118" s="26" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H119" s="26" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H120" s="26" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H121" s="26" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H122" s="26" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H123" s="26" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H124" s="26" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H125" s="26" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H126" s="26" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H127" s="26" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H128" s="26" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H129" s="26" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H130" s="26" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H131" s="26" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H132" s="26" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H133" s="26" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H134" s="26" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H135" s="26" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H136" s="26" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H137" s="26" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H138" s="26" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H139" s="26" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H140" s="26" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H141" s="26" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H142" s="26" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H143" s="26" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H144" s="26" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H145" s="26" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H146" s="26" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H147" s="26" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H148" s="26" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H149" s="26" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H150" s="26" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H151" s="26" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H152" s="26" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H153" s="26" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H154" s="26" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H155" s="26" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H156" s="26" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H157" s="26" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H158" s="26" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H159" s="26" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H160" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H161" s="26" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H162" s="26" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H163" s="26" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H164" s="26" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H165" s="26" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H166" s="26" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H167" s="26" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H168" s="26" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H169" s="26" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H170" s="26" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H171" s="26" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H172" s="26" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H173" s="26" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H174" s="26" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H175" s="26" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H176" s="26" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H177" s="26" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H178" s="26" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H179" s="26" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H180" s="26" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H181" s="26" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H182" s="26" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H183" s="26" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H184" s="26" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H185" s="26" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H186" s="26" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H187" s="26" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H188" s="26" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H189" s="26" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H190" s="26" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H191" s="26" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H192" s="26" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H193" s="26" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H194" s="26" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H195" s="26" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H196" s="26" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H197" s="26" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H198" s="26" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H199" s="26" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H200" s="26" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H201" s="26" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H202" s="26" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H203" s="26" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H204" s="26" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H205" s="26" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H206" s="26" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H207" s="26" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H208" s="26" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H209" s="26" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H210" s="26" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H211" s="26" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H212" s="26" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H213" s="26" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H214" s="26" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H215" s="26" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H216" s="26" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H217" s="26" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H218" s="26" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H219" s="26" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H220" s="26" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H221" s="26" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H222" s="26" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H223" s="26" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H224" s="26" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H225" s="26" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H226" s="26" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H227" s="26" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H228" s="26" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H229" s="26" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H230" s="26" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H231" s="26" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H232" s="26" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H233" s="26" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H234" s="26" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H235" s="26" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H236" s="26" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H237" s="26" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H238" s="26" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H239" s="26" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H240" s="26" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H241" s="26" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H242" s="26" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34704,7 +34716,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="53.04"/>
@@ -34712,10 +34724,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34723,7 +34735,7 @@
         <v>4203</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34731,7 +34743,7 @@
         <v>4203100001</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34739,7 +34751,7 @@
         <v>4203100009</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34747,7 +34759,7 @@
         <v>6106</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34755,7 +34767,7 @@
         <v>6106100000</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34763,7 +34775,7 @@
         <v>6106200000</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34771,7 +34783,7 @@
         <v>6106901000</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34779,7 +34791,7 @@
         <v>6106903000</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34787,7 +34799,7 @@
         <v>6106905000</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34795,7 +34807,7 @@
         <v>6106909000</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34803,7 +34815,7 @@
         <v>6201</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34811,7 +34823,7 @@
         <v>6201200000</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34819,7 +34831,7 @@
         <v>6201300000</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34827,7 +34839,7 @@
         <v>6201400000</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34835,7 +34847,7 @@
         <v>6201900000</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34843,7 +34855,7 @@
         <v>6202</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34851,7 +34863,7 @@
         <v>6202200000</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34859,7 +34871,7 @@
         <v>6202300000</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34867,7 +34879,7 @@
         <v>6202400001</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34875,7 +34887,7 @@
         <v>6202400009</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34883,7 +34895,7 @@
         <v>6202900001</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34891,7 +34903,7 @@
         <v>6202900009</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34899,7 +34911,7 @@
         <v>6302</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34907,7 +34919,7 @@
         <v>6302100001</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34915,7 +34927,7 @@
         <v>6302100009</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34923,7 +34935,7 @@
         <v>6302210000</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34931,7 +34943,7 @@
         <v>6302221000</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34939,7 +34951,7 @@
         <v>6302229000</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34947,7 +34959,7 @@
         <v>6302310001</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34955,7 +34967,7 @@
         <v>6302310009</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34963,7 +34975,7 @@
         <v>6302321000</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34971,7 +34983,7 @@
         <v>6302329000</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34979,7 +34991,7 @@
         <v>6302392001</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34987,7 +34999,7 @@
         <v>6302392009</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34995,7 +35007,7 @@
         <v>6302399000</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35003,7 +35015,7 @@
         <v>6302400000</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35011,7 +35023,7 @@
         <v>6302510001</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35019,7 +35031,7 @@
         <v>6302510009</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35027,7 +35039,7 @@
         <v>6302531000</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35035,7 +35047,7 @@
         <v>6302539000</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35043,7 +35055,7 @@
         <v>6302591000</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35051,7 +35063,7 @@
         <v>6302599000</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35059,7 +35071,7 @@
         <v>6302600000</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35067,7 +35079,7 @@
         <v>6302910000</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35075,7 +35087,7 @@
         <v>6302931000</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35083,7 +35095,7 @@
         <v>6302939000</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35091,7 +35103,7 @@
         <v>6302991000</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35099,7 +35111,7 @@
         <v>6302999000</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35107,7 +35119,7 @@
         <v>4303</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35115,7 +35127,7 @@
         <v>4303109010</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35123,7 +35135,7 @@
         <v>4303109020</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35131,7 +35143,7 @@
         <v>4303109030</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35139,7 +35151,7 @@
         <v>4303109040</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35147,7 +35159,7 @@
         <v>4303109050</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35155,7 +35167,7 @@
         <v>4303109060</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35163,7 +35175,7 @@
         <v>4303109080</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35171,7 +35183,7 @@
         <v>3303</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35179,7 +35191,7 @@
         <v>3303001000</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35187,7 +35199,7 @@
         <v>3303009000</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35195,7 +35207,7 @@
         <v>4011</v>
       </c>
       <c r="B61" s="33" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35203,7 +35215,7 @@
         <v>4011100003</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35211,7 +35223,7 @@
         <v>4011100009</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35219,7 +35231,7 @@
         <v>4011201000</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35227,7 +35239,7 @@
         <v>4011209000</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35235,7 +35247,7 @@
         <v>4011400000</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35243,7 +35255,7 @@
         <v>4011700000</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35251,7 +35263,7 @@
         <v>4011800000</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35259,7 +35271,7 @@
         <v>4011900000</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35267,7 +35279,7 @@
         <v>6401</v>
       </c>
       <c r="B70" s="33" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35275,7 +35287,7 @@
         <v>6401100000</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35283,7 +35295,7 @@
         <v>6401921000</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35291,7 +35303,7 @@
         <v>6401929000</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35299,7 +35311,7 @@
         <v>6401990000</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35307,7 +35319,7 @@
         <v>6402</v>
       </c>
       <c r="B75" s="33" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35315,7 +35327,7 @@
         <v>6402121000</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35323,7 +35335,7 @@
         <v>6402129000</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35331,7 +35343,7 @@
         <v>6402190000</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35339,7 +35351,7 @@
         <v>6402200000</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35347,7 +35359,7 @@
         <v>6402911000</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35355,7 +35367,7 @@
         <v>6402919000</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35363,7 +35375,7 @@
         <v>6402990500</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35371,7 +35383,7 @@
         <v>6402991000</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35379,7 +35391,7 @@
         <v>6402993100</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35387,7 +35399,7 @@
         <v>6402993900</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35395,7 +35407,7 @@
         <v>6402995000</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35403,7 +35415,7 @@
         <v>6402999100</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35411,7 +35423,7 @@
         <v>6402999300</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35419,7 +35431,7 @@
         <v>6402999600</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35427,7 +35439,7 @@
         <v>6402999800</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35435,7 +35447,7 @@
         <v>6403</v>
       </c>
       <c r="B91" s="33" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35443,7 +35455,7 @@
         <v>6403120000</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35451,7 +35463,7 @@
         <v>6403190000</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35459,7 +35471,7 @@
         <v>6403200000</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35467,7 +35479,7 @@
         <v>6403400000</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35475,7 +35487,7 @@
         <v>6403510500</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35483,7 +35495,7 @@
         <v>6403511100</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35491,7 +35503,7 @@
         <v>6403511500</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35499,7 +35511,7 @@
         <v>6403511900</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35507,7 +35519,7 @@
         <v>6403519100</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35515,7 +35527,7 @@
         <v>6403519500</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35523,7 +35535,7 @@
         <v>6403519900</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35531,7 +35543,7 @@
         <v>6403590500</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35539,7 +35551,7 @@
         <v>6403591100</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35547,7 +35559,7 @@
         <v>6403593100</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35555,7 +35567,7 @@
         <v>6403593500</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35563,7 +35575,7 @@
         <v>6403593900</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35571,7 +35583,7 @@
         <v>6403595000</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35579,7 +35591,7 @@
         <v>6403599100</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35587,7 +35599,7 @@
         <v>6403599500</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35595,7 +35607,7 @@
         <v>6403599900</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35603,7 +35615,7 @@
         <v>6403910500</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35611,7 +35623,7 @@
         <v>6403911100</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35619,7 +35631,7 @@
         <v>6403911300</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35627,7 +35639,7 @@
         <v>6403911600</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35635,7 +35647,7 @@
         <v>6403911800</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35643,7 +35655,7 @@
         <v>6403919100</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35651,7 +35663,7 @@
         <v>6403919300</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35659,7 +35671,7 @@
         <v>6403919600</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35667,7 +35679,7 @@
         <v>6403919800</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35675,7 +35687,7 @@
         <v>6403990500</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35683,7 +35695,7 @@
         <v>6403991100</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35691,7 +35703,7 @@
         <v>6403993100</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35699,7 +35711,7 @@
         <v>6403993300</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35707,7 +35719,7 @@
         <v>6403993600</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35715,7 +35727,7 @@
         <v>6403993800</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35723,7 +35735,7 @@
         <v>6403995000</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35731,7 +35743,7 @@
         <v>6403999100</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35739,7 +35751,7 @@
         <v>6403999300</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35747,7 +35759,7 @@
         <v>6403999600</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35755,7 +35767,7 @@
         <v>6403999800</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35763,7 +35775,7 @@
         <v>6404</v>
       </c>
       <c r="B132" s="33" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35771,7 +35783,7 @@
         <v>6404110000</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35779,7 +35791,7 @@
         <v>6404191000</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35787,7 +35799,7 @@
         <v>6404199000</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35795,7 +35807,7 @@
         <v>6404191000</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35803,7 +35815,7 @@
         <v>6404209000</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35811,7 +35823,7 @@
         <v>6405</v>
       </c>
       <c r="B138" s="33" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35819,7 +35831,7 @@
         <v>6405100001</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35827,7 +35839,7 @@
         <v>6405100009</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35835,7 +35847,7 @@
         <v>6405201000</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35843,7 +35855,7 @@
         <v>6405209100</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35851,7 +35863,7 @@
         <v>6405209900</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35859,7 +35871,7 @@
         <v>6405901000</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35867,7 +35879,7 @@
         <v>6405909000</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upd: - color added
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/белье_по каждому размеру.xlsx
+++ b/app/download_dir/system_files/белье_по каждому размеру.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="690">
   <si>
     <t xml:space="preserve">Код ТНВЭД</t>
   </si>
@@ -1270,6 +1270,9 @@
   </si>
   <si>
     <t xml:space="preserve">ЛЮКСЕМБУРГ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КАМУФЛЯЖНЫЙ</t>
   </si>
   <si>
     <t xml:space="preserve">МАВРИКИЙ</t>
@@ -3173,10 +3176,10 @@
   <dimension ref="A1:AMJ1780"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="65.42"/>
@@ -32720,11 +32723,11 @@
   </sheetPr>
   <dimension ref="A1:I243"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E111" activeCellId="0" sqref="E111"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E113" activeCellId="0" sqref="E113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="24.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="49.34"/>
@@ -34036,653 +34039,656 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E113" s="7" t="s">
+        <v>414</v>
+      </c>
       <c r="H113" s="26" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H114" s="26" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H115" s="26" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H116" s="26" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H117" s="26" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H118" s="26" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H119" s="26" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H120" s="26" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H121" s="26" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H122" s="26" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H123" s="26" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H124" s="26" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H125" s="26" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H126" s="26" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H127" s="26" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H128" s="26" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H129" s="26" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H130" s="26" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H131" s="26" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H132" s="26" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H133" s="26" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H134" s="26" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H135" s="26" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H136" s="26" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H137" s="26" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H138" s="26" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H139" s="26" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H140" s="26" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H141" s="26" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H142" s="26" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H143" s="26" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H144" s="26" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H145" s="26" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H146" s="26" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H147" s="26" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H148" s="26" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H149" s="26" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H150" s="26" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H151" s="26" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H152" s="26" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H153" s="26" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H154" s="26" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H155" s="26" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H156" s="26" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H157" s="26" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H158" s="26" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H159" s="26" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H160" s="26" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H161" s="26" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H162" s="26" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H163" s="26" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H164" s="26" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H165" s="26" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H166" s="26" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H167" s="26" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H168" s="26" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H169" s="26" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H170" s="26" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H171" s="26" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H172" s="26" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H173" s="26" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H174" s="26" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H175" s="26" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H176" s="26" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H177" s="26" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H178" s="26" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H179" s="26" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H180" s="26" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H181" s="26" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H182" s="26" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H183" s="26" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H184" s="26" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H185" s="26" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H186" s="26" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H187" s="26" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H188" s="26" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H189" s="26" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H190" s="26" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H191" s="26" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H192" s="26" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H193" s="26" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H194" s="26" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H195" s="26" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H196" s="26" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H197" s="26" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H198" s="26" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H199" s="26" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H200" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H201" s="26" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H202" s="26" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H203" s="26" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H204" s="26" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H205" s="26" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H206" s="26" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H207" s="26" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H208" s="26" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H209" s="26" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H210" s="26" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H211" s="26" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H212" s="26" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H213" s="26" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H214" s="26" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H215" s="26" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H216" s="26" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H217" s="26" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H218" s="26" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H219" s="26" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H220" s="26" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H221" s="26" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H222" s="26" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H223" s="26" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H224" s="26" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H225" s="26" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H226" s="26" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H227" s="26" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H228" s="26" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H229" s="26" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H230" s="26" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H231" s="26" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H232" s="26" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H233" s="26" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H234" s="26" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H235" s="26" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H236" s="26" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H237" s="26" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H238" s="26" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H239" s="26" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H240" s="26" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H241" s="26" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H242" s="26" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34692,7 +34698,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:E112">
+  <conditionalFormatting sqref="E2:E113">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -34716,7 +34722,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="53.04"/>
@@ -34724,10 +34730,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34735,7 +34741,7 @@
         <v>4203</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34743,7 +34749,7 @@
         <v>4203100001</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34751,7 +34757,7 @@
         <v>4203100009</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34759,7 +34765,7 @@
         <v>6106</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34767,7 +34773,7 @@
         <v>6106100000</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34775,7 +34781,7 @@
         <v>6106200000</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34783,7 +34789,7 @@
         <v>6106901000</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34791,7 +34797,7 @@
         <v>6106903000</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34799,7 +34805,7 @@
         <v>6106905000</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34807,7 +34813,7 @@
         <v>6106909000</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34815,7 +34821,7 @@
         <v>6201</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34823,7 +34829,7 @@
         <v>6201200000</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34831,7 +34837,7 @@
         <v>6201300000</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34839,7 +34845,7 @@
         <v>6201400000</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34847,7 +34853,7 @@
         <v>6201900000</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34855,7 +34861,7 @@
         <v>6202</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34863,7 +34869,7 @@
         <v>6202200000</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34871,7 +34877,7 @@
         <v>6202300000</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34879,7 +34885,7 @@
         <v>6202400001</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34887,7 +34893,7 @@
         <v>6202400009</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34895,7 +34901,7 @@
         <v>6202900001</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34903,7 +34909,7 @@
         <v>6202900009</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34911,7 +34917,7 @@
         <v>6302</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34919,7 +34925,7 @@
         <v>6302100001</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34927,7 +34933,7 @@
         <v>6302100009</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34935,7 +34941,7 @@
         <v>6302210000</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34943,7 +34949,7 @@
         <v>6302221000</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34951,7 +34957,7 @@
         <v>6302229000</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34959,7 +34965,7 @@
         <v>6302310001</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34967,7 +34973,7 @@
         <v>6302310009</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34975,7 +34981,7 @@
         <v>6302321000</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34983,7 +34989,7 @@
         <v>6302329000</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34991,7 +34997,7 @@
         <v>6302392001</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34999,7 +35005,7 @@
         <v>6302392009</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35007,7 +35013,7 @@
         <v>6302399000</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35015,7 +35021,7 @@
         <v>6302400000</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35023,7 +35029,7 @@
         <v>6302510001</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35031,7 +35037,7 @@
         <v>6302510009</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35039,7 +35045,7 @@
         <v>6302531000</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35047,7 +35053,7 @@
         <v>6302539000</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35055,7 +35061,7 @@
         <v>6302591000</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35063,7 +35069,7 @@
         <v>6302599000</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35071,7 +35077,7 @@
         <v>6302600000</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35079,7 +35085,7 @@
         <v>6302910000</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35087,7 +35093,7 @@
         <v>6302931000</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35095,7 +35101,7 @@
         <v>6302939000</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35103,7 +35109,7 @@
         <v>6302991000</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35111,7 +35117,7 @@
         <v>6302999000</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35119,7 +35125,7 @@
         <v>4303</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35127,7 +35133,7 @@
         <v>4303109010</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35135,7 +35141,7 @@
         <v>4303109020</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35143,7 +35149,7 @@
         <v>4303109030</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35151,7 +35157,7 @@
         <v>4303109040</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35159,7 +35165,7 @@
         <v>4303109050</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35167,7 +35173,7 @@
         <v>4303109060</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35175,7 +35181,7 @@
         <v>4303109080</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35183,7 +35189,7 @@
         <v>3303</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35191,7 +35197,7 @@
         <v>3303001000</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35199,7 +35205,7 @@
         <v>3303009000</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35207,7 +35213,7 @@
         <v>4011</v>
       </c>
       <c r="B61" s="33" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35215,7 +35221,7 @@
         <v>4011100003</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35223,7 +35229,7 @@
         <v>4011100009</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35231,7 +35237,7 @@
         <v>4011201000</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35239,7 +35245,7 @@
         <v>4011209000</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35247,7 +35253,7 @@
         <v>4011400000</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35255,7 +35261,7 @@
         <v>4011700000</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35263,7 +35269,7 @@
         <v>4011800000</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35271,7 +35277,7 @@
         <v>4011900000</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35279,7 +35285,7 @@
         <v>6401</v>
       </c>
       <c r="B70" s="33" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35287,7 +35293,7 @@
         <v>6401100000</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35295,7 +35301,7 @@
         <v>6401921000</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35303,7 +35309,7 @@
         <v>6401929000</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35311,7 +35317,7 @@
         <v>6401990000</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35319,7 +35325,7 @@
         <v>6402</v>
       </c>
       <c r="B75" s="33" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35327,7 +35333,7 @@
         <v>6402121000</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35335,7 +35341,7 @@
         <v>6402129000</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35343,7 +35349,7 @@
         <v>6402190000</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35351,7 +35357,7 @@
         <v>6402200000</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35359,7 +35365,7 @@
         <v>6402911000</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35367,7 +35373,7 @@
         <v>6402919000</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35375,7 +35381,7 @@
         <v>6402990500</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35383,7 +35389,7 @@
         <v>6402991000</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35391,7 +35397,7 @@
         <v>6402993100</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35399,7 +35405,7 @@
         <v>6402993900</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35407,7 +35413,7 @@
         <v>6402995000</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35415,7 +35421,7 @@
         <v>6402999100</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35423,7 +35429,7 @@
         <v>6402999300</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35431,7 +35437,7 @@
         <v>6402999600</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35439,7 +35445,7 @@
         <v>6402999800</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35447,7 +35453,7 @@
         <v>6403</v>
       </c>
       <c r="B91" s="33" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35455,7 +35461,7 @@
         <v>6403120000</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35463,7 +35469,7 @@
         <v>6403190000</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35471,7 +35477,7 @@
         <v>6403200000</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35479,7 +35485,7 @@
         <v>6403400000</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35487,7 +35493,7 @@
         <v>6403510500</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35495,7 +35501,7 @@
         <v>6403511100</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35503,7 +35509,7 @@
         <v>6403511500</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35511,7 +35517,7 @@
         <v>6403511900</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35519,7 +35525,7 @@
         <v>6403519100</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35527,7 +35533,7 @@
         <v>6403519500</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35535,7 +35541,7 @@
         <v>6403519900</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35543,7 +35549,7 @@
         <v>6403590500</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35551,7 +35557,7 @@
         <v>6403591100</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35559,7 +35565,7 @@
         <v>6403593100</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35567,7 +35573,7 @@
         <v>6403593500</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35575,7 +35581,7 @@
         <v>6403593900</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35583,7 +35589,7 @@
         <v>6403595000</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35591,7 +35597,7 @@
         <v>6403599100</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35599,7 +35605,7 @@
         <v>6403599500</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35607,7 +35613,7 @@
         <v>6403599900</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35615,7 +35621,7 @@
         <v>6403910500</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35623,7 +35629,7 @@
         <v>6403911100</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35631,7 +35637,7 @@
         <v>6403911300</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35639,7 +35645,7 @@
         <v>6403911600</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35647,7 +35653,7 @@
         <v>6403911800</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35655,7 +35661,7 @@
         <v>6403919100</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35663,7 +35669,7 @@
         <v>6403919300</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35671,7 +35677,7 @@
         <v>6403919600</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35679,7 +35685,7 @@
         <v>6403919800</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35687,7 +35693,7 @@
         <v>6403990500</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35695,7 +35701,7 @@
         <v>6403991100</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35703,7 +35709,7 @@
         <v>6403993100</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35711,7 +35717,7 @@
         <v>6403993300</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35719,7 +35725,7 @@
         <v>6403993600</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35727,7 +35733,7 @@
         <v>6403993800</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35735,7 +35741,7 @@
         <v>6403995000</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35743,7 +35749,7 @@
         <v>6403999100</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35751,7 +35757,7 @@
         <v>6403999300</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35759,7 +35765,7 @@
         <v>6403999600</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35767,7 +35773,7 @@
         <v>6403999800</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35775,7 +35781,7 @@
         <v>6404</v>
       </c>
       <c r="B132" s="33" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35783,7 +35789,7 @@
         <v>6404110000</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35791,7 +35797,7 @@
         <v>6404191000</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35799,7 +35805,7 @@
         <v>6404199000</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35807,7 +35813,7 @@
         <v>6404191000</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35815,7 +35821,7 @@
         <v>6404209000</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35823,7 +35829,7 @@
         <v>6405</v>
       </c>
       <c r="B138" s="33" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35831,7 +35837,7 @@
         <v>6405100001</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35839,7 +35845,7 @@
         <v>6405100009</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35847,7 +35853,7 @@
         <v>6405201000</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35855,7 +35861,7 @@
         <v>6405209100</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35863,7 +35869,7 @@
         <v>6405209900</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35871,7 +35877,7 @@
         <v>6405901000</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35879,7 +35885,7 @@
         <v>6405909000</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upd: - linen tables edit
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/белье_по каждому размеру.xlsx
+++ b/app/download_dir/system_files/белье_по каждому размеру.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="689">
   <si>
     <t xml:space="preserve">Код ТНВЭД</t>
   </si>
@@ -189,7 +189,7 @@
     <t xml:space="preserve">5gb</t>
   </si>
   <si>
-    <t xml:space="preserve">САЛФЕТКИ ДЛЯ СТЕКЛЯННОЙ ПОСУДЫ</t>
+    <t xml:space="preserve">ИЗДЕЛИЕ ДЛЯ БАНИ И САУНЫ</t>
   </si>
   <si>
     <t xml:space="preserve">КОФЕЙНЫЙ</t>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t xml:space="preserve">АВСТРАЛИЯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ИЗДЕЛИЕ ДЛЯ БАНИ И САУНЫ</t>
   </si>
   <si>
     <t xml:space="preserve">БЕЖЕВЫЙ/ЗЕЛЕНЫЙ</t>
@@ -3176,10 +3173,10 @@
   <dimension ref="A1:AMJ1780"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="65.42"/>
@@ -3582,7 +3579,7 @@
       </c>
       <c r="B7" s="15" t="str">
         <f aca="false">CONCATENATE(F7, " ", C7, " арт. ", E7, " цвет ", G7, ". ", J7)</f>
-        <v>САЛФЕТКИ ДЛЯ СТЕКЛЯННОЙ ПОСУДЫ Meerkat арт. 5gb цвет КОФЕЙНЫЙ. сатин</v>
+        <v>ИЗДЕЛИЕ ДЛЯ БАНИ И САУНЫ Meerkat арт. 5gb цвет КОФЕЙНЫЙ. сатин</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>50</v>
@@ -32727,7 +32724,7 @@
       <selection pane="topLeft" activeCell="E113" activeCellId="0" sqref="E113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="24.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="49.34"/>
@@ -32811,19 +32808,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="26" t="s">
         <v>93</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>94</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>73</v>
@@ -32831,425 +32828,425 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>56</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="26" t="s">
         <v>107</v>
-      </c>
-      <c r="H7" s="26" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>68</v>
       </c>
       <c r="G8" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="26" t="s">
         <v>111</v>
-      </c>
-      <c r="H8" s="26" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="26" t="s">
         <v>115</v>
-      </c>
-      <c r="H9" s="26" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="26" t="s">
         <v>119</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="H11" s="26" t="s">
         <v>123</v>
-      </c>
-      <c r="H11" s="26" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="H12" s="26" t="s">
         <v>127</v>
-      </c>
-      <c r="H12" s="26" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="26" t="s">
         <v>131</v>
-      </c>
-      <c r="H13" s="26" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="H14" s="26" t="s">
         <v>135</v>
-      </c>
-      <c r="H14" s="26" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="26" t="s">
         <v>139</v>
-      </c>
-      <c r="H15" s="26" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="H16" s="26" t="s">
         <v>145</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="G17" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="H17" s="26" t="s">
         <v>150</v>
-      </c>
-      <c r="H17" s="26" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="H18" s="26" t="s">
         <v>155</v>
-      </c>
-      <c r="H18" s="26" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="H19" s="26" t="s">
         <v>160</v>
-      </c>
-      <c r="H19" s="26" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="G20" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="H20" s="26" t="s">
         <v>164</v>
-      </c>
-      <c r="H20" s="26" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="H21" s="26" t="s">
         <v>168</v>
-      </c>
-      <c r="H21" s="26" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="H22" s="26" t="s">
         <v>172</v>
-      </c>
-      <c r="H22" s="26" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="H23" s="26" t="s">
         <v>176</v>
-      </c>
-      <c r="H23" s="26" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="G24" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="H24" s="26" t="s">
         <v>180</v>
-      </c>
-      <c r="H24" s="26" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="H25" s="26" t="s">
         <v>184</v>
-      </c>
-      <c r="H25" s="26" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="G26" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="H26" s="26" t="s">
         <v>188</v>
-      </c>
-      <c r="H26" s="26" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="H27" s="26" t="s">
         <v>192</v>
-      </c>
-      <c r="H27" s="26" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="G28" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="H28" s="26" t="s">
         <v>196</v>
-      </c>
-      <c r="H28" s="26" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="H29" s="26" t="s">
         <v>200</v>
-      </c>
-      <c r="H29" s="26" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="G30" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="H30" s="26" t="s">
         <v>204</v>
-      </c>
-      <c r="H30" s="26" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>54</v>
       </c>
       <c r="G31" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H31" s="26" t="s">
         <v>207</v>
-      </c>
-      <c r="H31" s="26" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33257,550 +33254,550 @@
         <v>67</v>
       </c>
       <c r="E32" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="G32" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="H32" s="26" t="s">
         <v>210</v>
-      </c>
-      <c r="H32" s="26" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="G33" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="H33" s="26" t="s">
         <v>214</v>
-      </c>
-      <c r="H33" s="26" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="G34" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="H34" s="26" t="s">
         <v>218</v>
-      </c>
-      <c r="H34" s="26" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D35" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="G35" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="H35" s="26" t="s">
         <v>222</v>
-      </c>
-      <c r="H35" s="26" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D36" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="G36" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="H36" s="26" t="s">
         <v>226</v>
-      </c>
-      <c r="H36" s="26" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D37" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="G37" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="H37" s="26" t="s">
         <v>230</v>
-      </c>
-      <c r="H37" s="26" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D38" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="G38" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="H38" s="26" t="s">
         <v>234</v>
-      </c>
-      <c r="H38" s="26" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D39" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="G39" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="H39" s="26" t="s">
         <v>238</v>
-      </c>
-      <c r="H39" s="26" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="G40" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="H40" s="26" t="s">
         <v>242</v>
-      </c>
-      <c r="H40" s="26" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D41" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="H41" s="26" t="s">
         <v>246</v>
-      </c>
-      <c r="H41" s="26" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="G42" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="H42" s="26" t="s">
         <v>249</v>
-      </c>
-      <c r="H42" s="26" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="G43" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="H43" s="26" t="s">
         <v>252</v>
-      </c>
-      <c r="H43" s="26" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="G44" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="H44" s="26" t="s">
         <v>255</v>
-      </c>
-      <c r="H44" s="26" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="G45" s="7" t="s">
+      <c r="H45" s="26" t="s">
         <v>258</v>
-      </c>
-      <c r="H45" s="26" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="G46" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="G46" s="7" t="s">
+      <c r="H46" s="26" t="s">
         <v>261</v>
-      </c>
-      <c r="H46" s="26" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E47" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="G47" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="H47" s="26" t="s">
         <v>264</v>
-      </c>
-      <c r="H47" s="26" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="G48" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="G48" s="7" t="s">
+      <c r="H48" s="26" t="s">
         <v>267</v>
-      </c>
-      <c r="H48" s="26" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E49" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="G49" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="H49" s="26" t="s">
         <v>270</v>
-      </c>
-      <c r="H49" s="26" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="G50" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="G50" s="7" t="s">
+      <c r="H50" s="26" t="s">
         <v>273</v>
-      </c>
-      <c r="H50" s="26" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G51" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="G51" s="7" t="s">
+      <c r="H51" s="26" t="s">
         <v>276</v>
-      </c>
-      <c r="H51" s="26" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="G52" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="G52" s="7" t="s">
+      <c r="H52" s="26" t="s">
         <v>279</v>
-      </c>
-      <c r="H52" s="26" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="G53" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="G53" s="7" t="s">
+      <c r="H53" s="26" t="s">
         <v>282</v>
-      </c>
-      <c r="H53" s="26" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="G54" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="G54" s="7" t="s">
+      <c r="H54" s="26" t="s">
         <v>285</v>
-      </c>
-      <c r="H54" s="26" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="G55" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="G55" s="7" t="s">
+      <c r="H55" s="26" t="s">
         <v>288</v>
-      </c>
-      <c r="H55" s="26" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E56" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="G56" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="G56" s="7" t="s">
+      <c r="H56" s="26" t="s">
         <v>291</v>
-      </c>
-      <c r="H56" s="26" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="G57" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="G57" s="7" t="s">
+      <c r="H57" s="26" t="s">
         <v>294</v>
-      </c>
-      <c r="H57" s="26" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="G58" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="G58" s="7" t="s">
+      <c r="H58" s="26" t="s">
         <v>297</v>
-      </c>
-      <c r="H58" s="26" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="G59" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="G59" s="7" t="s">
+      <c r="H59" s="26" t="s">
         <v>300</v>
-      </c>
-      <c r="H59" s="26" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="G60" s="7" t="s">
+      <c r="H60" s="26" t="s">
         <v>303</v>
-      </c>
-      <c r="H60" s="26" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="G61" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="G61" s="7" t="s">
+      <c r="H61" s="26" t="s">
         <v>306</v>
-      </c>
-      <c r="H61" s="26" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="G62" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="G62" s="7" t="s">
+      <c r="H62" s="26" t="s">
         <v>309</v>
-      </c>
-      <c r="H62" s="26" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G63" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="G63" s="7" t="s">
+      <c r="H63" s="26" t="s">
         <v>312</v>
-      </c>
-      <c r="H63" s="26" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="G64" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="G64" s="7" t="s">
+      <c r="H64" s="26" t="s">
         <v>315</v>
-      </c>
-      <c r="H64" s="26" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="G65" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="G65" s="7" t="s">
+      <c r="H65" s="26" t="s">
         <v>318</v>
-      </c>
-      <c r="H65" s="26" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E66" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="G66" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="G66" s="7" t="s">
+      <c r="H66" s="26" t="s">
         <v>321</v>
-      </c>
-      <c r="H66" s="26" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="G67" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="G67" s="7" t="s">
+      <c r="H67" s="26" t="s">
         <v>324</v>
-      </c>
-      <c r="H67" s="26" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="H68" s="26" t="s">
         <v>326</v>
-      </c>
-      <c r="H68" s="26" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E69" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="H69" s="26" t="s">
         <v>328</v>
-      </c>
-      <c r="H69" s="26" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="H70" s="26" t="s">
         <v>330</v>
-      </c>
-      <c r="H70" s="26" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E71" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="H71" s="26" t="s">
         <v>332</v>
-      </c>
-      <c r="H71" s="26" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="H72" s="26" t="s">
         <v>334</v>
-      </c>
-      <c r="H72" s="26" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="H73" s="26" t="s">
         <v>336</v>
-      </c>
-      <c r="H73" s="26" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="H74" s="26" t="s">
         <v>338</v>
-      </c>
-      <c r="H74" s="26" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E75" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="H75" s="26" t="s">
         <v>340</v>
-      </c>
-      <c r="H75" s="26" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="H76" s="26" t="s">
         <v>342</v>
-      </c>
-      <c r="H76" s="26" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E77" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="H77" s="26" t="s">
         <v>344</v>
-      </c>
-      <c r="H77" s="26" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E78" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="H78" s="26" t="s">
         <v>346</v>
-      </c>
-      <c r="H78" s="26" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E79" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="H79" s="26" t="s">
         <v>348</v>
-      </c>
-      <c r="H79" s="26" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="H80" s="26" t="s">
         <v>350</v>
-      </c>
-      <c r="H80" s="26" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E81" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="H81" s="26" t="s">
         <v>352</v>
-      </c>
-      <c r="H81" s="26" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E82" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="H82" s="26" t="s">
         <v>354</v>
-      </c>
-      <c r="H82" s="26" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H83" s="26" t="s">
         <v>72</v>
@@ -33808,103 +33805,103 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E84" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="H84" s="26" t="s">
         <v>357</v>
-      </c>
-      <c r="H84" s="26" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E85" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="H85" s="26" t="s">
         <v>359</v>
-      </c>
-      <c r="H85" s="26" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E86" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="H86" s="26" t="s">
         <v>361</v>
-      </c>
-      <c r="H86" s="26" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="H87" s="26" t="s">
         <v>363</v>
-      </c>
-      <c r="H87" s="26" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E88" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="H88" s="26" t="s">
         <v>365</v>
-      </c>
-      <c r="H88" s="26" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E89" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="H89" s="26" t="s">
         <v>367</v>
-      </c>
-      <c r="H89" s="26" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E90" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="H90" s="26" t="s">
         <v>369</v>
-      </c>
-      <c r="H90" s="26" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E91" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="H91" s="26" t="s">
         <v>371</v>
-      </c>
-      <c r="H91" s="26" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E92" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="H92" s="26" t="s">
         <v>373</v>
-      </c>
-      <c r="H92" s="26" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E93" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="H93" s="26" t="s">
         <v>375</v>
-      </c>
-      <c r="H93" s="26" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="H94" s="26" t="s">
         <v>377</v>
-      </c>
-      <c r="H94" s="26" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E95" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="H95" s="26" t="s">
         <v>379</v>
-      </c>
-      <c r="H95" s="26" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E96" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H96" s="26" t="s">
         <v>61</v>
@@ -33912,783 +33909,783 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E97" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="H97" s="26" t="s">
         <v>382</v>
-      </c>
-      <c r="H97" s="26" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E98" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="H98" s="26" t="s">
         <v>384</v>
-      </c>
-      <c r="H98" s="26" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E99" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="H99" s="26" t="s">
         <v>386</v>
-      </c>
-      <c r="H99" s="26" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="H100" s="26" t="s">
         <v>388</v>
-      </c>
-      <c r="H100" s="26" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E101" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="H101" s="26" t="s">
         <v>390</v>
-      </c>
-      <c r="H101" s="26" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E102" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="H102" s="26" t="s">
         <v>392</v>
-      </c>
-      <c r="H102" s="26" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E103" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="H103" s="26" t="s">
         <v>394</v>
-      </c>
-      <c r="H103" s="26" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E104" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="H104" s="26" t="s">
         <v>396</v>
-      </c>
-      <c r="H104" s="26" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E105" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="H105" s="26" t="s">
         <v>398</v>
-      </c>
-      <c r="H105" s="26" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E106" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="H106" s="26" t="s">
         <v>400</v>
-      </c>
-      <c r="H106" s="26" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E107" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="H107" s="26" t="s">
         <v>402</v>
-      </c>
-      <c r="H107" s="26" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E108" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="H108" s="26" t="s">
         <v>404</v>
-      </c>
-      <c r="H108" s="26" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H109" s="26" t="s">
         <v>406</v>
-      </c>
-      <c r="H109" s="26" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E110" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="H110" s="26" t="s">
         <v>408</v>
-      </c>
-      <c r="H110" s="26" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E111" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="H111" s="26" t="s">
         <v>410</v>
-      </c>
-      <c r="H111" s="26" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E112" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H112" s="26" t="s">
         <v>412</v>
-      </c>
-      <c r="H112" s="26" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E113" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="H113" s="26" t="s">
         <v>414</v>
-      </c>
-      <c r="H113" s="26" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H114" s="26" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H115" s="26" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H116" s="26" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H117" s="26" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H118" s="26" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H119" s="26" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H120" s="26" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H121" s="26" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H122" s="26" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H123" s="26" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H124" s="26" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H125" s="26" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H126" s="26" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H127" s="26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H128" s="26" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H129" s="26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H130" s="26" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H131" s="26" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H132" s="26" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H133" s="26" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H134" s="26" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H135" s="26" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H136" s="26" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H137" s="26" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H138" s="26" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H139" s="26" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H140" s="26" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H141" s="26" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H142" s="26" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H143" s="26" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H144" s="26" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H145" s="26" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H146" s="26" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H147" s="26" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H148" s="26" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H149" s="26" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H150" s="26" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H151" s="26" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H152" s="26" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H153" s="26" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H154" s="26" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H155" s="26" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H156" s="26" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H157" s="26" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H158" s="26" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H159" s="26" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H160" s="26" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H161" s="26" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H162" s="26" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H163" s="26" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H164" s="26" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H165" s="26" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H166" s="26" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H167" s="26" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H168" s="26" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H169" s="26" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H170" s="26" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H171" s="26" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H172" s="26" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H173" s="26" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H174" s="26" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H175" s="26" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H176" s="26" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H177" s="26" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H178" s="26" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H179" s="26" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H180" s="26" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H181" s="26" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H182" s="26" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H183" s="26" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H184" s="26" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H185" s="26" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H186" s="26" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H187" s="26" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H188" s="26" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H189" s="26" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H190" s="26" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H191" s="26" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H192" s="26" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H193" s="26" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H194" s="26" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H195" s="26" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H196" s="26" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H197" s="26" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H198" s="26" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H199" s="26" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H200" s="26" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H201" s="26" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H202" s="26" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H203" s="26" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H204" s="26" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H205" s="26" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H206" s="26" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H207" s="26" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H208" s="26" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H209" s="26" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H210" s="26" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H211" s="26" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H212" s="26" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H213" s="26" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H214" s="26" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H215" s="26" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H216" s="26" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H217" s="26" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H218" s="26" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H219" s="26" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H220" s="26" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H221" s="26" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H222" s="26" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H223" s="26" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H224" s="26" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H225" s="26" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H226" s="26" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H227" s="26" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H228" s="26" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H229" s="26" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H230" s="26" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H231" s="26" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H232" s="26" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H233" s="26" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H234" s="26" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H235" s="26" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H236" s="26" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H237" s="26" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H238" s="26" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H239" s="26" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H240" s="26" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H241" s="26" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H242" s="26" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34722,7 +34719,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="53.04"/>
@@ -34730,10 +34727,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
+        <v>544</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>545</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34741,7 +34738,7 @@
         <v>4203</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34749,7 +34746,7 @@
         <v>4203100001</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34757,7 +34754,7 @@
         <v>4203100009</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34765,7 +34762,7 @@
         <v>6106</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34773,7 +34770,7 @@
         <v>6106100000</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34781,7 +34778,7 @@
         <v>6106200000</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34789,7 +34786,7 @@
         <v>6106901000</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34797,7 +34794,7 @@
         <v>6106903000</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34805,7 +34802,7 @@
         <v>6106905000</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34813,7 +34810,7 @@
         <v>6106909000</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34821,7 +34818,7 @@
         <v>6201</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34829,7 +34826,7 @@
         <v>6201200000</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34837,7 +34834,7 @@
         <v>6201300000</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34845,7 +34842,7 @@
         <v>6201400000</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34853,7 +34850,7 @@
         <v>6201900000</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34861,7 +34858,7 @@
         <v>6202</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34869,7 +34866,7 @@
         <v>6202200000</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34877,7 +34874,7 @@
         <v>6202300000</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34885,7 +34882,7 @@
         <v>6202400001</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34893,7 +34890,7 @@
         <v>6202400009</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34901,7 +34898,7 @@
         <v>6202900001</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34909,7 +34906,7 @@
         <v>6202900009</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34917,7 +34914,7 @@
         <v>6302</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34925,7 +34922,7 @@
         <v>6302100001</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34933,7 +34930,7 @@
         <v>6302100009</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34941,7 +34938,7 @@
         <v>6302210000</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34949,7 +34946,7 @@
         <v>6302221000</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34957,7 +34954,7 @@
         <v>6302229000</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34965,7 +34962,7 @@
         <v>6302310001</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34973,7 +34970,7 @@
         <v>6302310009</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34981,7 +34978,7 @@
         <v>6302321000</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34989,7 +34986,7 @@
         <v>6302329000</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34997,7 +34994,7 @@
         <v>6302392001</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35005,7 +35002,7 @@
         <v>6302392009</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35013,7 +35010,7 @@
         <v>6302399000</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35021,7 +35018,7 @@
         <v>6302400000</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35029,7 +35026,7 @@
         <v>6302510001</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35037,7 +35034,7 @@
         <v>6302510009</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35045,7 +35042,7 @@
         <v>6302531000</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35053,7 +35050,7 @@
         <v>6302539000</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35061,7 +35058,7 @@
         <v>6302591000</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35069,7 +35066,7 @@
         <v>6302599000</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35077,7 +35074,7 @@
         <v>6302600000</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35085,7 +35082,7 @@
         <v>6302910000</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35093,7 +35090,7 @@
         <v>6302931000</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35101,7 +35098,7 @@
         <v>6302939000</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35109,7 +35106,7 @@
         <v>6302991000</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35117,7 +35114,7 @@
         <v>6302999000</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35125,7 +35122,7 @@
         <v>4303</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35133,7 +35130,7 @@
         <v>4303109010</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35141,7 +35138,7 @@
         <v>4303109020</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35149,7 +35146,7 @@
         <v>4303109030</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35157,7 +35154,7 @@
         <v>4303109040</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35165,7 +35162,7 @@
         <v>4303109050</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35173,7 +35170,7 @@
         <v>4303109060</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35181,7 +35178,7 @@
         <v>4303109080</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35189,7 +35186,7 @@
         <v>3303</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35197,7 +35194,7 @@
         <v>3303001000</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35205,7 +35202,7 @@
         <v>3303009000</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35213,7 +35210,7 @@
         <v>4011</v>
       </c>
       <c r="B61" s="33" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35221,7 +35218,7 @@
         <v>4011100003</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35229,7 +35226,7 @@
         <v>4011100009</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35237,7 +35234,7 @@
         <v>4011201000</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35245,7 +35242,7 @@
         <v>4011209000</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35253,7 +35250,7 @@
         <v>4011400000</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35261,7 +35258,7 @@
         <v>4011700000</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35269,7 +35266,7 @@
         <v>4011800000</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35277,7 +35274,7 @@
         <v>4011900000</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35285,7 +35282,7 @@
         <v>6401</v>
       </c>
       <c r="B70" s="33" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35293,7 +35290,7 @@
         <v>6401100000</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35301,7 +35298,7 @@
         <v>6401921000</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35309,7 +35306,7 @@
         <v>6401929000</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35317,7 +35314,7 @@
         <v>6401990000</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35325,7 +35322,7 @@
         <v>6402</v>
       </c>
       <c r="B75" s="33" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35333,7 +35330,7 @@
         <v>6402121000</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35341,7 +35338,7 @@
         <v>6402129000</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35349,7 +35346,7 @@
         <v>6402190000</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35357,7 +35354,7 @@
         <v>6402200000</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35365,7 +35362,7 @@
         <v>6402911000</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35373,7 +35370,7 @@
         <v>6402919000</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35381,7 +35378,7 @@
         <v>6402990500</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35389,7 +35386,7 @@
         <v>6402991000</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35397,7 +35394,7 @@
         <v>6402993100</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35405,7 +35402,7 @@
         <v>6402993900</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35413,7 +35410,7 @@
         <v>6402995000</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35421,7 +35418,7 @@
         <v>6402999100</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35429,7 +35426,7 @@
         <v>6402999300</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35437,7 +35434,7 @@
         <v>6402999600</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35445,7 +35442,7 @@
         <v>6402999800</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35453,7 +35450,7 @@
         <v>6403</v>
       </c>
       <c r="B91" s="33" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35461,7 +35458,7 @@
         <v>6403120000</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35469,7 +35466,7 @@
         <v>6403190000</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35477,7 +35474,7 @@
         <v>6403200000</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35485,7 +35482,7 @@
         <v>6403400000</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35493,7 +35490,7 @@
         <v>6403510500</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35501,7 +35498,7 @@
         <v>6403511100</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35509,7 +35506,7 @@
         <v>6403511500</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35517,7 +35514,7 @@
         <v>6403511900</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35525,7 +35522,7 @@
         <v>6403519100</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35533,7 +35530,7 @@
         <v>6403519500</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35541,7 +35538,7 @@
         <v>6403519900</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35549,7 +35546,7 @@
         <v>6403590500</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35557,7 +35554,7 @@
         <v>6403591100</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35565,7 +35562,7 @@
         <v>6403593100</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35573,7 +35570,7 @@
         <v>6403593500</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35581,7 +35578,7 @@
         <v>6403593900</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35589,7 +35586,7 @@
         <v>6403595000</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35597,7 +35594,7 @@
         <v>6403599100</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35605,7 +35602,7 @@
         <v>6403599500</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35613,7 +35610,7 @@
         <v>6403599900</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35621,7 +35618,7 @@
         <v>6403910500</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35629,7 +35626,7 @@
         <v>6403911100</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35637,7 +35634,7 @@
         <v>6403911300</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35645,7 +35642,7 @@
         <v>6403911600</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35653,7 +35650,7 @@
         <v>6403911800</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35661,7 +35658,7 @@
         <v>6403919100</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35669,7 +35666,7 @@
         <v>6403919300</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35677,7 +35674,7 @@
         <v>6403919600</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35685,7 +35682,7 @@
         <v>6403919800</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35693,7 +35690,7 @@
         <v>6403990500</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35701,7 +35698,7 @@
         <v>6403991100</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35709,7 +35706,7 @@
         <v>6403993100</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35717,7 +35714,7 @@
         <v>6403993300</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35725,7 +35722,7 @@
         <v>6403993600</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35733,7 +35730,7 @@
         <v>6403993800</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35741,7 +35738,7 @@
         <v>6403995000</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35749,7 +35746,7 @@
         <v>6403999100</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35757,7 +35754,7 @@
         <v>6403999300</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35765,7 +35762,7 @@
         <v>6403999600</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35773,7 +35770,7 @@
         <v>6403999800</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35781,7 +35778,7 @@
         <v>6404</v>
       </c>
       <c r="B132" s="33" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35789,7 +35786,7 @@
         <v>6404110000</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35797,7 +35794,7 @@
         <v>6404191000</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35805,7 +35802,7 @@
         <v>6404199000</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35813,7 +35810,7 @@
         <v>6404191000</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35821,7 +35818,7 @@
         <v>6404209000</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35829,7 +35826,7 @@
         <v>6405</v>
       </c>
       <c r="B138" s="33" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35837,7 +35834,7 @@
         <v>6405100001</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35845,7 +35842,7 @@
         <v>6405100009</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35853,7 +35850,7 @@
         <v>6405201000</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35861,7 +35858,7 @@
         <v>6405209100</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35869,7 +35866,7 @@
         <v>6405209900</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35877,7 +35874,7 @@
         <v>6405901000</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35885,7 +35882,7 @@
         <v>6405909000</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>